<commit_message>
feat: updated files and new pdf_parser
</commit_message>
<xml_diff>
--- a/docs/template-dcm.xlsx
+++ b/docs/template-dcm.xlsx
@@ -1050,9 +1050,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010069EA7952651B2E4C8ABE43C1505E70C4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="477863cacb66906565f0ad6600a82b1c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e1ca75-8d70-4c07-a1d5-008ce9de9a75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac3c32d1535fc2015dbe5c10975a053b" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010069EA7952651B2E4C8ABE43C1505E70C4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bec2e83585562a3f58cfd26f5d451141">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e1ca75-8d70-4c07-a1d5-008ce9de9a75" xmlns:ns3="6182920f-9004-47cb-8729-6f79319a1e85" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d227f7d82698ea555e402e5c53adbb68" ns2:_="" ns3:_="">
     <xsd:import namespace="b6e1ca75-8d70-4c07-a1d5-008ce9de9a75"/>
+    <xsd:import namespace="6182920f-9004-47cb-8729-6f79319a1e85"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1070,6 +1071,8 @@
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1137,6 +1140,36 @@
     <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6182920f-9004-47cb-8729-6f79319a1e85" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1255,7 +1288,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19DBF2D1-9B40-49A4-8167-22949B2D5755}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03A4B196-7136-4CF2-A25B-A33654795FF1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>